<commit_message>
Changed the generichelper with the try catch of element finding logic
</commit_message>
<xml_diff>
--- a/TestData/KD.xlsx
+++ b/TestData/KD.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\anushri.mundada\source\repos\SeleniumProject\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{717C757E-4182-4945-8A1F-2B66724164E9}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB35A9C3-FC8A-402B-BCB9-7116D6DDB858}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="57480" yWindow="4575" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-53" yWindow="-53" windowWidth="25706" windowHeight="13906" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ClinicianLanding" sheetId="2" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="52">
   <si>
     <t>Keyword</t>
   </si>
@@ -175,17 +175,20 @@
     <t>img[alt='Citadel Health Pty. Ltd.']</t>
   </si>
   <si>
-    <t>Compare and get text</t>
-  </si>
-  <si>
     <t>Compare</t>
+  </si>
+  <si>
+    <t>Compare the patient name</t>
+  </si>
+  <si>
+    <t>SM2ITHEE, Sophia</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -208,6 +211,13 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color rgb="FF363636"/>
+      <name val="Open Sans"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="3">
@@ -252,13 +262,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -543,7 +554,7 @@
   <dimension ref="A1:F19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E22" sqref="E22"/>
+      <selection activeCell="F19" sqref="F19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -885,15 +896,15 @@
       </c>
       <c r="F18" s="2"/>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:6" ht="15.75" x14ac:dyDescent="0.3">
       <c r="A19" s="2" t="s">
         <v>46</v>
       </c>
       <c r="B19" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="C19" s="2" t="s">
         <v>49</v>
-      </c>
-      <c r="C19" s="2" t="s">
-        <v>50</v>
       </c>
       <c r="D19" s="2" t="s">
         <v>37</v>
@@ -901,7 +912,9 @@
       <c r="E19" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="F19" s="2"/>
+      <c r="F19" s="4" t="s">
+        <v>51</v>
+      </c>
     </row>
   </sheetData>
   <hyperlinks>

</xml_diff>